<commit_message>
More program added to the Testcase
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
   <si>
     <t>Firstname</t>
   </si>
@@ -32,34 +32,160 @@
     <t>Lastname</t>
   </si>
   <si>
-    <t>Vin</t>
-  </si>
-  <si>
     <t>Mileage</t>
   </si>
   <si>
     <t>JN8AS58TX9W905001</t>
   </si>
   <si>
-    <t>Automation</t>
-  </si>
-  <si>
     <t>Test</t>
   </si>
   <si>
-    <t>program</t>
-  </si>
-  <si>
-    <t>Used Vehicle - SNL</t>
-  </si>
-  <si>
-    <t>Surcharge</t>
-  </si>
-  <si>
-    <t>3VWDZ7AJ7BM373945</t>
-  </si>
-  <si>
-    <t>Absolute Reserve Care Plus - RR1</t>
+    <t>2T1BR18E5WC056406</t>
+  </si>
+  <si>
+    <t>Limited Warranty - RAW</t>
+  </si>
+  <si>
+    <t>VIN</t>
+  </si>
+  <si>
+    <t>programs</t>
+  </si>
+  <si>
+    <t>Essentials</t>
+  </si>
+  <si>
+    <t>Limited Warranty</t>
+  </si>
+  <si>
+    <t>Limited Warranty - OCW</t>
+  </si>
+  <si>
+    <t>Powertrain Plus - PTP</t>
+  </si>
+  <si>
+    <t>Sentinel Program - QCU</t>
+  </si>
+  <si>
+    <t>Service Drive - SDF</t>
+  </si>
+  <si>
+    <t>Used Vechicle - RNL</t>
+  </si>
+  <si>
+    <t>Used Vechicle - SNE</t>
+  </si>
+  <si>
+    <t>Used Vechicle - SNF</t>
+  </si>
+  <si>
+    <t>Used Vechicle - SNI</t>
+  </si>
+  <si>
+    <t>Used Vechicle - SNL</t>
+  </si>
+  <si>
+    <t>Used Vechicle - SPK</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Auto Test</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Automation 1</t>
+  </si>
+  <si>
+    <t>Automation 2</t>
+  </si>
+  <si>
+    <t>Automation 3</t>
+  </si>
+  <si>
+    <t>Automation 4</t>
+  </si>
+  <si>
+    <t>Automation 5</t>
+  </si>
+  <si>
+    <t>Automation 6</t>
+  </si>
+  <si>
+    <t>Automation 7</t>
+  </si>
+  <si>
+    <t>Automation 8</t>
+  </si>
+  <si>
+    <t>Automation 9</t>
+  </si>
+  <si>
+    <t>Automation 10</t>
+  </si>
+  <si>
+    <t>Automation 11</t>
+  </si>
+  <si>
+    <t>Automation 12</t>
+  </si>
+  <si>
+    <t>Automation 13</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>Test 2</t>
+  </si>
+  <si>
+    <t>Test 3</t>
+  </si>
+  <si>
+    <t>Test 4</t>
+  </si>
+  <si>
+    <t>Test 5</t>
+  </si>
+  <si>
+    <t>Test 6</t>
+  </si>
+  <si>
+    <t>Test 7</t>
+  </si>
+  <si>
+    <t>Test 8</t>
+  </si>
+  <si>
+    <t>Test 9</t>
+  </si>
+  <si>
+    <t>Test 10</t>
+  </si>
+  <si>
+    <t>Test 11</t>
+  </si>
+  <si>
+    <t>Test 12</t>
+  </si>
+  <si>
+    <t>Test 13</t>
+  </si>
+  <si>
+    <t>GenerateContract</t>
+  </si>
+  <si>
+    <t>one</t>
   </si>
 </sst>
 </file>
@@ -95,8 +221,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,78 +504,472 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="3" width="11.21875" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="31.109375" customWidth="1"/>
+    <col min="6" max="6" width="29.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="8" max="9" width="16.77734375" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2">
+        <v>2345</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2">
+        <v>45678</v>
+      </c>
+      <c r="J2">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3">
+        <v>2345</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3">
+        <v>45678</v>
+      </c>
+      <c r="J3">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>2345</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4">
+        <v>45678</v>
+      </c>
+      <c r="J4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5">
+        <v>2345</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>123</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5">
+        <v>45678</v>
+      </c>
+      <c r="J5">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6">
+        <v>2345</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6">
+        <v>45678</v>
+      </c>
+      <c r="J6">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7">
+        <v>2345</v>
+      </c>
+      <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>1234</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7">
+        <v>45678</v>
+      </c>
+      <c r="J7">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>2345</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8">
+        <v>45678</v>
+      </c>
+      <c r="J8">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>2345</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9">
+        <v>45678</v>
+      </c>
+      <c r="J9">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10">
+        <v>2345</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10">
+        <v>45678</v>
+      </c>
+      <c r="J10">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11">
+        <v>2345</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11">
+        <v>45678</v>
+      </c>
+      <c r="J11">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12">
+        <v>2345</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12">
+        <v>45678</v>
+      </c>
+      <c r="J12">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13">
+        <v>2345</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13">
+        <v>45678</v>
+      </c>
+      <c r="J13">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14">
+        <v>2345</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14">
+        <v>45678</v>
+      </c>
+      <c r="J14">
+        <v>9999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More program added to the test script
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Firstname</t>
   </si>
@@ -44,9 +44,6 @@
     <t>2T1BR18E5WC056406</t>
   </si>
   <si>
-    <t>Limited Warranty - RAW</t>
-  </si>
-  <si>
     <t>VIN</t>
   </si>
   <si>
@@ -71,24 +68,6 @@
     <t>Service Drive - SDF</t>
   </si>
   <si>
-    <t>Used Vechicle - RNL</t>
-  </si>
-  <si>
-    <t>Used Vechicle - SNE</t>
-  </si>
-  <si>
-    <t>Used Vechicle - SNF</t>
-  </si>
-  <si>
-    <t>Used Vechicle - SNI</t>
-  </si>
-  <si>
-    <t>Used Vechicle - SNL</t>
-  </si>
-  <si>
-    <t>Used Vechicle - SPK</t>
-  </si>
-  <si>
     <t>Last Name</t>
   </si>
   <si>
@@ -113,9 +92,6 @@
     <t>Automation 3</t>
   </si>
   <si>
-    <t>Automation 4</t>
-  </si>
-  <si>
     <t>Automation 5</t>
   </si>
   <si>
@@ -125,24 +101,6 @@
     <t>Automation 7</t>
   </si>
   <si>
-    <t>Automation 8</t>
-  </si>
-  <si>
-    <t>Automation 9</t>
-  </si>
-  <si>
-    <t>Automation 10</t>
-  </si>
-  <si>
-    <t>Automation 11</t>
-  </si>
-  <si>
-    <t>Automation 12</t>
-  </si>
-  <si>
-    <t>Automation 13</t>
-  </si>
-  <si>
     <t>Test 1</t>
   </si>
   <si>
@@ -152,9 +110,6 @@
     <t>Test 3</t>
   </si>
   <si>
-    <t>Test 4</t>
-  </si>
-  <si>
     <t>Test 5</t>
   </si>
   <si>
@@ -162,24 +117,6 @@
   </si>
   <si>
     <t>Test 7</t>
-  </si>
-  <si>
-    <t>Test 8</t>
-  </si>
-  <si>
-    <t>Test 9</t>
-  </si>
-  <si>
-    <t>Test 10</t>
-  </si>
-  <si>
-    <t>Test 11</t>
-  </si>
-  <si>
-    <t>Test 12</t>
-  </si>
-  <si>
-    <t>Test 13</t>
   </si>
   <si>
     <t>GenerateContract</t>
@@ -504,18 +441,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.21875" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" customWidth="1"/>
     <col min="5" max="5" width="31.109375" customWidth="1"/>
     <col min="6" max="6" width="29.21875" customWidth="1"/>
     <col min="7" max="7" width="13.5546875" customWidth="1"/>
@@ -531,55 +468,55 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2">
         <v>2345</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I2">
         <v>45678</v>
@@ -590,28 +527,28 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
         <v>2345</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I3">
         <v>45678</v>
@@ -620,30 +557,30 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
         <v>2345</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I4">
         <v>45678</v>
@@ -654,28 +591,28 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
         <v>2345</v>
       </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I5">
         <v>45678</v>
@@ -686,28 +623,28 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
         <v>2345</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="G6" t="s">
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I6">
         <v>45678</v>
@@ -718,257 +655,33 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7">
         <v>2345</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I7">
         <v>45678</v>
       </c>
       <c r="J7">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8">
-        <v>2345</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8">
-        <v>45678</v>
-      </c>
-      <c r="J8">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9">
-        <v>2345</v>
-      </c>
-      <c r="D9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9">
-        <v>45678</v>
-      </c>
-      <c r="J9">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10">
-        <v>2345</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10">
-        <v>45678</v>
-      </c>
-      <c r="J10">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11">
-        <v>2345</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11">
-        <v>45678</v>
-      </c>
-      <c r="J11">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12">
-        <v>2345</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12">
-        <v>45678</v>
-      </c>
-      <c r="J12">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13">
-        <v>2345</v>
-      </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13">
-        <v>45678</v>
-      </c>
-      <c r="J13">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14">
-        <v>2345</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14">
-        <v>45678</v>
-      </c>
-      <c r="J14">
         <v>9999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Generate Contract Test Cases added
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Firstname</t>
   </si>
@@ -38,9 +38,6 @@
     <t>JN8AS58TX9W905001</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
     <t>2T1BR18E5WC056406</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>Service Drive - SDF</t>
   </si>
   <si>
-    <t>Last Name</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -123,6 +117,9 @@
   </si>
   <si>
     <t>one</t>
+  </si>
+  <si>
+    <t>Surcharge</t>
   </si>
 </sst>
 </file>
@@ -444,7 +441,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD12"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,8 +451,7 @@
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="11.21875" customWidth="1"/>
     <col min="5" max="5" width="31.109375" customWidth="1"/>
-    <col min="6" max="6" width="29.21875" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="6" max="7" width="29.21875" customWidth="1"/>
     <col min="8" max="9" width="16.77734375" customWidth="1"/>
     <col min="10" max="10" width="15.109375" customWidth="1"/>
   </cols>
@@ -468,37 +464,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>14</v>
+      <c r="G1" t="s">
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -507,16 +503,16 @@
         <v>2345</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I2">
         <v>45678</v>
@@ -527,28 +523,28 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>2345</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I3">
         <v>45678</v>
@@ -559,10 +555,10 @@
     </row>
     <row r="4" spans="1:11" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -571,16 +567,16 @@
         <v>2345</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I4">
         <v>45678</v>
@@ -591,10 +587,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -603,16 +599,16 @@
         <v>2345</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I5">
         <v>45678</v>
@@ -623,28 +619,28 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6">
         <v>2345</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I6">
         <v>45678</v>
@@ -655,10 +651,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -667,16 +663,16 @@
         <v>2345</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I7">
         <v>45678</v>

</xml_diff>

<commit_message>
validate PDF contract Test Cases added
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUL\Workspace\ADL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17088" windowHeight="7788"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17388" windowHeight="3444"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -441,7 +437,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added more test data
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="52">
   <si>
     <t>Firstname</t>
   </si>
@@ -122,29 +122,79 @@
     <t>program2</t>
   </si>
   <si>
-    <t>1HGCV1F31NA005121</t>
-  </si>
-  <si>
     <t>Automation 8</t>
   </si>
   <si>
     <t>Test 8</t>
   </si>
   <si>
-    <t>Absolute Reserve Care Lease</t>
+    <t>5J6RW2H89NA004619</t>
+  </si>
+  <si>
+    <t>Used Vehicle - RNL</t>
+  </si>
+  <si>
+    <t>Used Vehicle - SNI</t>
+  </si>
+  <si>
+    <t>Automation 9</t>
+  </si>
+  <si>
+    <t>Test 9</t>
+  </si>
+  <si>
+    <t>Used Vehicle - SNE</t>
+  </si>
+  <si>
+    <t>Used Vehicle - SNL</t>
+  </si>
+  <si>
+    <t>Automation 10</t>
+  </si>
+  <si>
+    <t>Test 10</t>
+  </si>
+  <si>
+    <t>Used Vehicle - SNF</t>
+  </si>
+  <si>
+    <t>Used Vehicle - SPK</t>
+  </si>
+  <si>
+    <t>Automation 11</t>
+  </si>
+  <si>
+    <t>Test 11</t>
+  </si>
+  <si>
+    <t>Automation 12</t>
+  </si>
+  <si>
+    <t>Test 12</t>
+  </si>
+  <si>
+    <t>Automation 13</t>
+  </si>
+  <si>
+    <t>Test 13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="MuseoSans-300"/>
     </font>
   </fonts>
   <fills count="2">
@@ -167,9 +217,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,13 +503,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -468,7 +521,7 @@
     <col min="10" max="10" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +554,7 @@
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -533,7 +586,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -565,7 +618,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="13.9" customHeight="1">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -597,7 +650,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="13.5" customHeight="1">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -629,7 +682,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -661,7 +714,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -693,35 +746,195 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:11" customFormat="1">
+      <c r="A8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8">
-        <v>112</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="D8" s="3">
+        <v>2345</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8">
-        <v>45678</v>
-      </c>
-      <c r="J8">
+      <c r="F8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="3">
+        <v>45678</v>
+      </c>
+      <c r="J8" s="3">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2345</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="3">
+        <v>45678</v>
+      </c>
+      <c r="J9" s="3">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2345</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="3">
+        <v>45678</v>
+      </c>
+      <c r="J10" s="3">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2345</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="3">
+        <v>45678</v>
+      </c>
+      <c r="J11" s="3">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2345</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="3">
+        <v>45678</v>
+      </c>
+      <c r="J12" s="3">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2345</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="3">
+        <v>45678</v>
+      </c>
+      <c r="J13" s="3">
         <v>9999999</v>
       </c>
     </row>
@@ -733,21 +946,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
     <col min="6" max="6" width="27.140625" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -782,7 +996,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -817,7 +1031,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -852,7 +1066,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -887,7 +1101,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -922,7 +1136,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="6" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" customFormat="1">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -957,7 +1171,111 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="7" spans="1:11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:11" customFormat="1">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7">
+        <v>2345</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7">
+        <v>45678</v>
+      </c>
+      <c r="K7">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <v>2345</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <v>45678</v>
+      </c>
+      <c r="K8">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9">
+        <v>2345</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9">
+        <v>45678</v>
+      </c>
+      <c r="K9">
+        <v>9999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Quote History code committed
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23175" windowHeight="10695"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14736" windowHeight="5520"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="56">
   <si>
     <t>Firstname</t>
   </si>
@@ -177,6 +177,18 @@
   </si>
   <si>
     <t>Test 6</t>
+  </si>
+  <si>
+    <t>New Vehicle - NSC</t>
+  </si>
+  <si>
+    <t>5FNRL6H27NB019645</t>
+  </si>
+  <si>
+    <t>Test 14</t>
+  </si>
+  <si>
+    <t>Automation 14</t>
   </si>
 </sst>
 </file>
@@ -510,22 +522,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:J13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.140625" customWidth="1"/>
-    <col min="6" max="7" width="29.28515625" customWidth="1"/>
-    <col min="8" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.109375" customWidth="1"/>
+    <col min="6" max="7" width="29.33203125" customWidth="1"/>
+    <col min="8" max="9" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -561,7 +573,7 @@
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" customFormat="1">
+    <row r="2" spans="1:11">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -593,7 +605,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="3" spans="1:11" customFormat="1">
+    <row r="3" spans="1:11">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -625,7 +637,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="4" spans="1:11" customFormat="1">
+    <row r="4" spans="1:11">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -657,7 +669,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" customFormat="1">
+    <row r="5" spans="1:11">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -689,7 +701,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="6" spans="1:11" customFormat="1">
+    <row r="6" spans="1:11">
       <c r="A6" s="4" t="s">
         <v>50</v>
       </c>
@@ -721,7 +733,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="7" spans="1:11" customFormat="1">
+    <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -753,7 +765,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" customFormat="1">
+    <row r="8" spans="1:11">
       <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
@@ -785,7 +797,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="9" spans="1:11" customFormat="1">
+    <row r="9" spans="1:11">
       <c r="A9" s="4" t="s">
         <v>36</v>
       </c>
@@ -817,7 +829,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="10" spans="1:11" customFormat="1">
+    <row r="10" spans="1:11">
       <c r="A10" s="4" t="s">
         <v>40</v>
       </c>
@@ -849,7 +861,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="11" spans="1:11" customFormat="1">
+    <row r="11" spans="1:11">
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
@@ -881,7 +893,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="12" spans="1:11" customFormat="1">
+    <row r="12" spans="1:11">
       <c r="A12" s="4" t="s">
         <v>46</v>
       </c>
@@ -913,7 +925,7 @@
         <v>9999999</v>
       </c>
     </row>
-    <row r="13" spans="1:11" customFormat="1">
+    <row r="13" spans="1:11">
       <c r="A13" s="4" t="s">
         <v>48</v>
       </c>
@@ -942,6 +954,38 @@
         <v>45678</v>
       </c>
       <c r="J13" s="4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="4">
+        <v>123</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J14" s="4">
         <v>9999999</v>
       </c>
     </row>
@@ -959,13 +1003,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="27.109375" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">

</xml_diff>

<commit_message>
Screenshot added in the test suite
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14736" windowHeight="5520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12828" windowHeight="4992"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -524,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Web Contract by Dealer Test cases
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUL\Workspace\ADL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17724" windowHeight="7788"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22176" windowHeight="7788"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
     <sheet name="Two_program" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="B4:H28"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="61">
   <si>
     <t>Firstname</t>
   </si>
@@ -193,6 +189,21 @@
   </si>
   <si>
     <t>Automation 14</t>
+  </si>
+  <si>
+    <t>Unlimited Time - AUN</t>
+  </si>
+  <si>
+    <t>Lifetime Warranty - New</t>
+  </si>
+  <si>
+    <t>Test 15</t>
+  </si>
+  <si>
+    <t>Absolute Reserve Care Lease</t>
+  </si>
+  <si>
+    <t>Automation 15</t>
   </si>
 </sst>
 </file>
@@ -240,9 +251,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -527,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -546,451 +558,484 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:11" s="6" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J2" s="4">
+        <v>9999999</v>
+      </c>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3">
-        <v>2345</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D3" s="4">
+        <v>2345</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="3">
-        <v>45678</v>
-      </c>
-      <c r="J2" s="3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="3" t="s">
+      <c r="F3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J3" s="4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="3">
-        <v>2345</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D4" s="4">
+        <v>2345</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="3">
-        <v>45678</v>
-      </c>
-      <c r="J3" s="3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="3" t="s">
+      <c r="F4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J4" s="4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="3">
-        <v>2345</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D5" s="4">
+        <v>2345</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="3">
-        <v>45678</v>
-      </c>
-      <c r="J4" s="3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="3" t="s">
+      <c r="F5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J5" s="4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3">
-        <v>2345</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D6" s="4">
+        <v>2345</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="3">
-        <v>45678</v>
-      </c>
-      <c r="J5" s="3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="3" t="s">
+      <c r="F6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J6" s="4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3">
-        <v>2345</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D7" s="4">
+        <v>2345</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="3">
-        <v>45678</v>
-      </c>
-      <c r="J6" s="3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="3" t="s">
+      <c r="F7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J7" s="4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="3">
-        <v>2345</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D8" s="4">
+        <v>2345</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="3">
-        <v>45678</v>
-      </c>
-      <c r="J7" s="3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="3" t="s">
+      <c r="F8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J8" s="4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="3">
-        <v>2345</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D9" s="4">
+        <v>2345</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="3">
-        <v>45678</v>
-      </c>
-      <c r="J8" s="3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="3" t="s">
+      <c r="F9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J9" s="4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="3">
-        <v>2345</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D10" s="4">
+        <v>2345</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="3">
-        <v>45678</v>
-      </c>
-      <c r="J9" s="3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="3" t="s">
+      <c r="F10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J10" s="4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="3">
-        <v>2345</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D11" s="4">
+        <v>2345</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="3">
-        <v>45678</v>
-      </c>
-      <c r="J10" s="3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="3" t="s">
+      <c r="F11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J11" s="4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="3">
-        <v>2345</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D12" s="4">
+        <v>2345</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="3">
-        <v>45678</v>
-      </c>
-      <c r="J11" s="3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="3" t="s">
+      <c r="F12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J12" s="4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="3">
-        <v>2345</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="D13" s="4">
+        <v>2345</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="3">
-        <v>45678</v>
-      </c>
-      <c r="J12" s="3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="3" t="s">
+      <c r="F13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J13" s="4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="3">
-        <v>2345</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="D14" s="4">
+        <v>2345</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="3">
-        <v>45678</v>
-      </c>
-      <c r="J13" s="3">
-        <v>9999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="3" t="s">
+      <c r="F14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J14" s="4">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D15" s="4">
         <v>123</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E15" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="3">
-        <v>45678</v>
-      </c>
-      <c r="J14" s="3">
+      <c r="F15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="4">
+        <v>45678</v>
+      </c>
+      <c r="J15" s="4">
         <v>9999999</v>
       </c>
     </row>
@@ -1002,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F9:F10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1053,107 +1098,177 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="13.8" customHeight="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4">
-        <v>2345</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="5">
+        <v>2345</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="4">
-        <v>45678</v>
-      </c>
-      <c r="K2" s="4">
+      <c r="G2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="5">
+        <v>45678</v>
+      </c>
+      <c r="K2" s="5">
         <v>9999999</v>
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5">
-        <v>2345</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="6">
+        <v>2345</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="5">
-        <v>45678</v>
-      </c>
-      <c r="K3" s="5">
+      <c r="G3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="6">
+        <v>45678</v>
+      </c>
+      <c r="K3" s="6">
         <v>9999999</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5">
-        <v>2345</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="6">
+        <v>2345</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="5">
-        <v>45678</v>
-      </c>
-      <c r="K4" s="5">
+      <c r="G4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="6">
+        <v>45678</v>
+      </c>
+      <c r="K4" s="6">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>2345</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5">
+        <v>45678</v>
+      </c>
+      <c r="K5">
+        <v>9999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6">
+        <v>2345</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>45678</v>
+      </c>
+      <c r="K6">
         <v>9999999</v>
       </c>
     </row>

</xml_diff>